<commit_message>
Added the stop node
</commit_message>
<xml_diff>
--- a/src/data/Excel Files/candidate_details_excel.xlsx
+++ b/src/data/Excel Files/candidate_details_excel.xlsx
@@ -5,15 +5,15 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\WebSamples\React Samples\react-workflow-automation\src\data\Excel Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C09CC38D-D932-4ED9-9F4C-A90510061DC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C35FE62-E318-4811-B30B-BF250286383B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{C17ABDC1-834C-4752-B3D2-C3B31F61D27C}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Candidates Data" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,10 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
-  <si>
-    <t>S.No</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
   <si>
     <t>Name</t>
   </si>
@@ -144,6 +141,18 @@
   </si>
   <si>
     <t>MBA (Operations)</t>
+  </si>
+  <si>
+    <t>Start Date</t>
+  </si>
+  <si>
+    <t>Acceptance Date</t>
+  </si>
+  <si>
+    <t>Salary (Annual)</t>
+  </si>
+  <si>
+    <t>S No</t>
   </si>
 </sst>
 </file>
@@ -187,7 +196,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -196,6 +205,9 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -532,10 +544,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12BF5F6B-E015-4AA3-B93D-3C0454C8A169}">
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:I11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -546,41 +558,53 @@
     <col min="4" max="4" width="19.90625" style="2" customWidth="1"/>
     <col min="5" max="5" width="17.36328125" style="2" customWidth="1"/>
     <col min="6" max="6" width="17.1796875" style="2" customWidth="1"/>
-    <col min="7" max="16384" width="8.7265625" style="2"/>
+    <col min="7" max="7" width="16.26953125" style="2" customWidth="1"/>
+    <col min="8" max="8" width="21.26953125" style="2" customWidth="1"/>
+    <col min="9" max="9" width="14" style="2" customWidth="1"/>
+    <col min="10" max="16384" width="8.7265625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" s="2">
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="D2" s="2" t="s">
         <v>7</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>8</v>
       </c>
       <c r="E2" s="3">
         <v>0.89</v>
@@ -588,19 +612,28 @@
       <c r="F2" s="3">
         <v>0.85</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G2" s="4">
+        <v>45992</v>
+      </c>
+      <c r="H2" s="4">
+        <v>45981</v>
+      </c>
+      <c r="I2" s="2">
+        <v>650000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" s="2">
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="D3" s="2" t="s">
         <v>10</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>11</v>
       </c>
       <c r="E3" s="3">
         <v>0.92</v>
@@ -608,19 +641,28 @@
       <c r="F3" s="3">
         <v>0.88</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G3" s="4">
+        <v>45996</v>
+      </c>
+      <c r="H3" s="4">
+        <v>45983</v>
+      </c>
+      <c r="I3" s="2">
+        <v>580000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" s="2">
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="D4" s="2" t="s">
         <v>13</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>14</v>
       </c>
       <c r="E4" s="3">
         <v>0.87</v>
@@ -628,19 +670,28 @@
       <c r="F4" s="3">
         <v>0.82</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G4" s="4">
+        <v>45994</v>
+      </c>
+      <c r="H4" s="4">
+        <v>45982</v>
+      </c>
+      <c r="I4" s="2">
+        <v>520000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" s="2">
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="D5" s="2" t="s">
         <v>16</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>17</v>
       </c>
       <c r="E5" s="3">
         <v>0.9</v>
@@ -648,19 +699,28 @@
       <c r="F5" s="3">
         <v>0.86</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G5" s="4">
+        <v>46001</v>
+      </c>
+      <c r="H5" s="4">
+        <v>45986</v>
+      </c>
+      <c r="I5" s="2">
+        <v>600000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" s="2">
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="D6" s="2" t="s">
         <v>19</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>20</v>
       </c>
       <c r="E6" s="3">
         <v>0.85</v>
@@ -668,19 +728,28 @@
       <c r="F6" s="3">
         <v>0.8</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G6" s="4">
+        <v>45998</v>
+      </c>
+      <c r="H6" s="4">
+        <v>45984</v>
+      </c>
+      <c r="I6" s="2">
+        <v>570000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" s="2">
         <v>6</v>
       </c>
       <c r="B7" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="D7" s="2" t="s">
         <v>22</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>23</v>
       </c>
       <c r="E7" s="3">
         <v>0.88</v>
@@ -688,19 +757,28 @@
       <c r="F7" s="3">
         <v>0.84</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G7" s="4">
+        <v>46003</v>
+      </c>
+      <c r="H7" s="4">
+        <v>45987</v>
+      </c>
+      <c r="I7" s="2">
+        <v>620000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8" s="2">
         <v>7</v>
       </c>
       <c r="B8" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="D8" s="2" t="s">
         <v>25</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>26</v>
       </c>
       <c r="E8" s="3">
         <v>0.86</v>
@@ -708,19 +786,28 @@
       <c r="F8" s="3">
         <v>0.81</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G8" s="4">
+        <v>45999</v>
+      </c>
+      <c r="H8" s="4">
+        <v>45985</v>
+      </c>
+      <c r="I8" s="2">
+        <v>500000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9" s="2">
         <v>8</v>
       </c>
       <c r="B9" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C9" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="D9" s="2" t="s">
         <v>28</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>29</v>
       </c>
       <c r="E9" s="3">
         <v>0.91</v>
@@ -728,19 +815,28 @@
       <c r="F9" s="3">
         <v>0.87</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G9" s="4">
+        <v>46006</v>
+      </c>
+      <c r="H9" s="4">
+        <v>45989</v>
+      </c>
+      <c r="I9" s="2">
+        <v>640000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10" s="2">
         <v>9</v>
       </c>
       <c r="B10" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C10" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="D10" s="2" t="s">
         <v>31</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>32</v>
       </c>
       <c r="E10" s="3">
         <v>0.93</v>
@@ -748,19 +844,28 @@
       <c r="F10" s="3">
         <v>0.89</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G10" s="4">
+        <v>46009</v>
+      </c>
+      <c r="H10" s="4">
+        <v>45991</v>
+      </c>
+      <c r="I10" s="2">
+        <v>720000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A11" s="2">
         <v>10</v>
       </c>
       <c r="B11" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C11" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="D11" s="2" t="s">
         <v>34</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>35</v>
       </c>
       <c r="E11" s="3">
         <v>0.9</v>
@@ -768,8 +873,18 @@
       <c r="F11" s="3">
         <v>0.85</v>
       </c>
+      <c r="G11" s="4">
+        <v>46011</v>
+      </c>
+      <c r="H11" s="4">
+        <v>45992</v>
+      </c>
+      <c r="I11" s="2">
+        <v>800000</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>